<commit_message>
Add task table and change user_id type to TEXT
</commit_message>
<xml_diff>
--- a/sql/mcd.xlsx
+++ b/sql/mcd.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSO\HS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSO\HS\hodor\Hodor\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MCD" sheetId="1" r:id="rId1"/>
-    <sheet name="ws_status" sheetId="2" r:id="rId2"/>
-    <sheet name="module_type" sheetId="3" r:id="rId3"/>
-    <sheet name="ship_type" sheetId="4" r:id="rId4"/>
+    <sheet name="task_type" sheetId="5" r:id="rId2"/>
+    <sheet name="ws_status" sheetId="2" r:id="rId3"/>
+    <sheet name="module_type" sheetId="3" r:id="rId4"/>
+    <sheet name="ship_type" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>user</t>
   </si>
@@ -213,14 +214,43 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>user_corpo</t>
+  </si>
+  <si>
+    <t>task_type</t>
+  </si>
+  <si>
+    <t>WS_BS</t>
+  </si>
+  <si>
+    <t>WS_TS</t>
+  </si>
+  <si>
+    <t>WS_FS</t>
+  </si>
+  <si>
+    <t>URGENT</t>
+  </si>
+  <si>
+    <t>DIVERS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -248,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -260,6 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,8 +309,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G7:G9" totalsRowShown="0">
-  <autoFilter ref="G7:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G7:G10" totalsRowShown="0">
+  <autoFilter ref="G7:G10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="user"/>
   </tableColumns>
@@ -338,8 +369,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B7:B13" totalsRowShown="0">
-  <autoFilter ref="B7:B13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B7:B14" totalsRowShown="0">
+  <autoFilter ref="B7:B14"/>
   <tableColumns count="1">
     <tableColumn id="1" name="task"/>
   </tableColumns>
@@ -642,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,8 +684,8 @@
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
@@ -823,6 +854,9 @@
       <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="G10" t="s">
+        <v>62</v>
+      </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
@@ -870,6 +904,9 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
@@ -956,6 +993,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1020,7 +1113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1075,7 +1168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>